<commit_message>
Tabellentrennung IST _ Plan aufgenommen
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B36A1-DFFE-4D1A-B161-C8A187768228}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D39915-90CB-49CD-B31E-F968D8B3B975}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -318,8 +318,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -11668,7 +11668,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>result.fBuchungsjournal</a:t>
+            <a:t>result.fBuchungsjournal_Plan</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13234,15 +13234,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
+      <xdr:colOff>361948</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>647699</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -13257,8 +13257,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6610349" y="11420474"/>
-          <a:ext cx="2352675" cy="2495551"/>
+          <a:off x="6610348" y="11420474"/>
+          <a:ext cx="4095751" cy="3048001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13306,7 +13306,20 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t> Werte werden in das Buchungsjournal geladen mit</a:t>
+            <a:t> Werte werden in das Buchungsjournal geladen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> result.fBuchungsjournal_IST</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -13461,6 +13474,78 @@
             </a:rPr>
             <a:t>Der PLAN - IST Vergleich erfolgt dann immer über die Sachkonten und Kostenstellenhierarchie</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="900" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Es ist nicht die selbe Tabelle wie das Plan Buchungsjournal um:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- IST separat nachts zu laden</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- IST mit TRUNCATE statt DELETE löschen zu können</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- PLAN bei den Neuberechnungen mit TRUNCATE statt DELETE zu löschen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="900" b="0" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -40019,20 +40104,20 @@
       <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -40042,10 +40127,10 @@
         <v>36</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
@@ -40066,36 +40151,41 @@
         <v>37</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="D13" s="12"/>
+      <c r="D13" s="11"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="12"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="10"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="11"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="12"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="10"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="11"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="12"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="11"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="12"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="10"/>
-      <c r="D17" s="12"/>
+      <c r="D17" s="11"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C13:D13"/>
@@ -40104,11 +40194,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40220,8 +40305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update testen und dbo.Main in Best Practice
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19512934-A4E5-4ADE-A258-A18E6AA1E15A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1517F35-05BA-44F4-A31E-06B11A2FE641}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
   <si>
     <t>Monitoring</t>
   </si>
@@ -496,6 +496,24 @@
   <si>
     <t>einheitliche Methodik über viele Projekte hinweg</t>
   </si>
+  <si>
+    <t>Mitwirkungspflichten des Kunden definieren</t>
+  </si>
+  <si>
+    <t>Der Kunde sollte das System testen - und dazu auch explizit verpflichtet werden. Mit einer Testliste und Erledigungsprotokoll</t>
+  </si>
+  <si>
+    <t>dbo.Main</t>
+  </si>
+  <si>
+    <t>alle Funktionalität sollte in der Prozedur dbo.Main enden - wenn man diese (nachts) aufruft, aktualisiert sich das gesamte System</t>
+  </si>
+  <si>
+    <t>dieser ruft typischer staging.spMain, load.spMain, import.spMain, calc.spMain auf, welche dann die Unterprozeduren enthalten.</t>
+  </si>
+  <si>
+    <t>Idealeweise kann man staging…..calc pro Modul getrennt laufen lassen</t>
+  </si>
 </sst>
 </file>
 
@@ -653,15 +671,15 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1335,8 +1353,8 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1352,7 +1370,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11277600" y="2038350"/>
-          <a:ext cx="4933950" cy="1885950"/>
+          <a:ext cx="4933950" cy="1619250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -43367,10 +43385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE89A27-A0F0-4951-A5E1-991F8FA81B66}">
-  <dimension ref="B1:D55"/>
+  <dimension ref="B1:D62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -43416,7 +43434,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -43446,168 +43464,201 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="14" t="s">
         <v>114</v>
       </c>
     </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D19" s="14"/>
+    </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" s="10" t="s">
-        <v>82</v>
+      <c r="C20" s="1" t="s">
+        <v>129</v>
       </c>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="10"/>
-      <c r="C21" s="1" t="s">
-        <v>115</v>
+      <c r="D21" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" s="10"/>
-      <c r="D22" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="D22" s="14"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B23" s="10"/>
-      <c r="D23" s="17" t="s">
-        <v>99</v>
+      <c r="B23" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="10"/>
-      <c r="D24" s="17"/>
+      <c r="C24" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="10"/>
-      <c r="D25" s="17"/>
+      <c r="D25" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="C26" s="1" t="s">
-        <v>83</v>
+      <c r="B26" s="10"/>
+      <c r="D26" s="14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D27" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="B27" s="10"/>
+      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="D28" s="1" t="s">
-        <v>85</v>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D33" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D33" s="17" t="s">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D35" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C36" s="1" t="s">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C37" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D37" s="1" t="s">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C40" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D40" s="1" t="s">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D41" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D41" s="17" t="s">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D42" s="14" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D42" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D43" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="D44" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="C45" s="1" t="s">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C46" s="1" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
-      <c r="D46" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D49" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D50" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D51" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B53" s="10" t="s">
-        <v>91</v>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D52" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C54" s="1" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D55" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D56" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D57" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B60" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="C61" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="D62" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -43792,23 +43843,23 @@
       <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="8"/>
@@ -43817,11 +43868,11 @@
       <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="8"/>
@@ -43841,37 +43892,42 @@
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="16"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C14" s="14"/>
-      <c r="D14" s="16"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C15" s="14"/>
-      <c r="D15" s="16"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C16" s="14"/>
-      <c r="D16" s="16"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="16"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.45">
-      <c r="C17" s="14"/>
-      <c r="D17" s="16"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="16"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C13:D13"/>
@@ -43880,11 +43936,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -44040,13 +44091,13 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="N11" s="20" t="s">
+      <c r="N11" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="P11" s="20" t="s">
+      <c r="P11" s="17" t="s">
         <v>68</v>
       </c>
     </row>
@@ -44065,10 +44116,10 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="16" t="s">
         <v>107</v>
       </c>
     </row>
@@ -44079,10 +44130,10 @@
       <c r="N16" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="O16" s="18">
+      <c r="O16" s="15">
         <v>2013</v>
       </c>
-      <c r="P16" s="18" t="s">
+      <c r="P16" s="15" t="s">
         <v>103</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test / MultiVPN in Doku
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1517F35-05BA-44F4-A31E-06B11A2FE641}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1542ECE5-0D4A-4A82-9D55-0497E7CD59EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BestPracticeWorkflow" sheetId="22" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="136">
   <si>
     <t>Monitoring</t>
   </si>
@@ -514,6 +514,9 @@
   <si>
     <t>Idealeweise kann man staging…..calc pro Modul getrennt laufen lassen</t>
   </si>
+  <si>
+    <t>mehrere Zugänge</t>
+  </si>
 </sst>
 </file>
 
@@ -678,8 +681,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -21776,7 +21779,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>http://Coplan:5000/[ClusterName]</a:t>
+            <a:t>http://[Server]:5000/[ClusterName]</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="900" baseline="0">
             <a:solidFill>
@@ -21961,7 +21964,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>Linked Server: SQL2, SQL1</a:t>
+            <a:t>Linked Server: SQLX</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="900" baseline="0">
             <a:solidFill>
@@ -22115,21 +22118,16 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>User: DataFactory</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="de-DE" sz="900" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="85000"/>
-                  <a:lumOff val="15000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(Leserechte)</a:t>
-          </a:r>
+            <a:t>User: DataFactory\saxess</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="900" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="de-DE" sz="900" baseline="0">
@@ -22461,15 +22459,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22484,8 +22482,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4038600" y="5629275"/>
-          <a:ext cx="1971675" cy="600075"/>
+          <a:off x="3810000" y="6410325"/>
+          <a:ext cx="1857375" cy="638175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22547,6 +22545,458 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Textfeld 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2AD8138-ACEB-4289-8A65-236733399108}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3781424" y="5553075"/>
+          <a:ext cx="4695825" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Benutzer</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Domäne\saxess  - das</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> ist unser Entwicklungsuser mit Adminrechten, Passwort läuft nie ab</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Domäne\FactoryService - ein einfacher Domänenbenutzer, KEIN Admin JEMALS IRGENDWO, PW läuft nie ab</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>AD Gruppe "DataFactoryUser" o.ä. anlegen und im SQL Server für DataFactory berechtigen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Der Zugriff</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> auf alle Vorsystem sollte mit dem User saxess erfolgen.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800101</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Textfeld 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93CB4B8A-05B5-4696-B6B9-98BF66A48978}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6076950" y="8896350"/>
+          <a:ext cx="2771776" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Testsystem / Produktivsystem</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mehrere</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Parallele Datenbanken</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Probleme:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Alle</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Scripte mit harten Referenzen funktionieren  ggf. nicht</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2143126</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Textfeld 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52590095-F3EC-40BD-9A74-2AAA0B0FA285}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11144250" y="8829675"/>
+          <a:ext cx="3838576" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Mehrere VPN Zugänge</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- Github</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> pro User installieren</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- ein Repo als Master definieren (von dort nimmt Powershell etc. die Scripte)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>- alle anderen Repos sind wie lokale Testumgebungen zu führen</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Probleme:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>mehrere</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> User können nicht gleichzeitig ein lokales Repo bearbeiten</a:t>
+          </a:r>
           <a:endParaRPr lang="de-DE" sz="800">
             <a:solidFill>
               <a:srgbClr val="203864"/>
@@ -43387,277 +43837,277 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE89A27-A0F0-4951-A5E1-991F8FA81B66}">
   <dimension ref="B1:D62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D10" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>129</v>
       </c>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="D25" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="D26" s="14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D41" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D42" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
         <v>95</v>
       </c>
@@ -43677,18 +44127,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43702,18 +44152,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
@@ -43732,18 +44182,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
   </sheetData>
@@ -43760,18 +44210,18 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
@@ -43790,19 +44240,19 @@
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>77</v>
       </c>
@@ -43822,62 +44272,62 @@
       <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>38</v>
       </c>
@@ -43888,46 +44338,41 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
+      <c r="D13" s="20"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="19"/>
+      <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
+      <c r="D14" s="20"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="19"/>
+      <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
+      <c r="D15" s="20"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="19"/>
+      <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="D16" s="20"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
+      <c r="D17" s="20"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C13:D13"/>
@@ -43936,6 +44381,11 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43951,18 +44401,18 @@
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
@@ -43982,19 +44432,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
@@ -44008,40 +44458,40 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="3" width="4.1328125" customWidth="1"/>
-    <col min="13" max="13" width="16.73046875" customWidth="1"/>
-    <col min="14" max="14" width="21.265625" customWidth="1"/>
-    <col min="15" max="15" width="33.86328125" customWidth="1"/>
-    <col min="16" max="16" width="48.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="15" max="15" width="33.85546875" customWidth="1"/>
+    <col min="16" max="16" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M5" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M6" s="11"/>
       <c r="N6" s="11" t="s">
         <v>52</v>
@@ -44053,7 +44503,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
@@ -44068,7 +44518,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
         <v>59</v>
       </c>
@@ -44076,103 +44526,108 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="M10" s="13" t="s">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M11" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N11" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="N11" s="17" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O12" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P12" s="17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="M13" s="13" t="s">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M14" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="N14" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="O13" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="P13" s="12" t="s">
+      <c r="P14" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="O14" s="16" t="s">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="P14" s="16" t="s">
+      <c r="P15" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
-      <c r="M16" s="13" t="s">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="M17" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N17" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="O16" s="15">
+      <c r="O17" s="15">
         <v>2013</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P17" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.45">
-      <c r="M18" s="13" t="s">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D19" s="4"/>
+      <c r="M19" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="N19" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="O18" s="12" t="s">
+      <c r="O19" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="P18" s="12" t="s">
+      <c r="P19" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.45">
-      <c r="D19" s="4"/>
-      <c r="N19" t="s">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
         <v>67</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O20" t="s">
         <v>67</v>
       </c>
-      <c r="P19" t="s">
+      <c r="P20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.45">
-      <c r="N20" t="s">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.45">
-      <c r="N21" t="s">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N22" t="s">
         <v>69</v>
       </c>
-      <c r="P21" t="s">
+      <c r="P22" t="s">
         <v>104</v>
       </c>
     </row>
@@ -44191,24 +44646,24 @@
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="Q2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:21" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:21" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -44216,13 +44671,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="Q4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>20</v>
       </c>
@@ -44230,7 +44685,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>21</v>
       </c>
@@ -44238,7 +44693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>22</v>
       </c>
@@ -44246,7 +44701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>26</v>
       </c>
@@ -44254,7 +44709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R10" t="s">
         <v>28</v>
       </c>
@@ -44262,67 +44717,67 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="51" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="55" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="56" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P56" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="57" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="58" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="61" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="63" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="64" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P65" t="s">
         <v>50</v>
       </c>
@@ -44342,79 +44797,79 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" style="1"/>
-    <col min="4" max="4" width="32.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.73046875" style="1"/>
-    <col min="8" max="8" width="43.86328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.73046875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.73046875" style="1" customWidth="1"/>
-    <col min="11" max="16" width="10.73046875" style="1"/>
-    <col min="17" max="19" width="5.86328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.59765625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.59765625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.86328125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.265625" style="1" customWidth="1"/>
-    <col min="24" max="26" width="10.73046875" style="1"/>
-    <col min="27" max="27" width="13.59765625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="32.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="1"/>
+    <col min="8" max="8" width="43.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16" width="10.7109375" style="1"/>
+    <col min="17" max="19" width="5.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="1" customWidth="1"/>
+    <col min="24" max="26" width="10.7109375" style="1"/>
+    <col min="27" max="27" width="13.5703125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="1"/>
     <col min="29" max="29" width="12" style="1" customWidth="1"/>
-    <col min="30" max="37" width="10.73046875" style="1"/>
+    <col min="30" max="37" width="10.7109375" style="1"/>
     <col min="38" max="38" width="16" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="10.73046875" style="1"/>
+    <col min="39" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:33" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AG7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG12" s="1" t="s">
         <v>14</v>
       </c>
@@ -44434,156 +44889,156 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
-    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U86" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U87" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U88" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G175" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Logo in Doku ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E789735C-B03D-4509-8E90-3AF32E75429E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05587397-1CA5-46E4-A8D5-EF8A1B095C46}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BestPracticeWorkflow" sheetId="22" r:id="rId1"/>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="lblAuftraggeber">ProjektOrga!$C$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -14779,6 +14779,156 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>87995</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37419A1B-2D77-42B1-B067-A86BE5167F1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2314575" y="5676900"/>
+          <a:ext cx="685800" cy="707120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>170208</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Grafik 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE28EE9-0F72-4C31-8E98-33A68DA7B902}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228725" y="5695950"/>
+          <a:ext cx="666750" cy="579783"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>459457</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26F2DB5F-40E9-41B3-805C-5F89D0220DEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2828926" y="6391275"/>
+          <a:ext cx="345156" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -38832,273 +38982,273 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D10" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D17" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D18" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="D25" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="D26" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D35" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D38" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D41" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D42" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D44" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D48" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D57" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C61" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1" t="s">
         <v>94</v>
       </c>
@@ -39118,18 +39268,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
@@ -39148,18 +39298,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
   </sheetData>
@@ -39176,18 +39326,18 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
@@ -39202,28 +39352,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748EB88F-C287-42AC-A455-699A81E8AA37}">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
@@ -39235,7 +39385,7 @@
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
@@ -39245,10 +39395,10 @@
       <c r="F8" s="19"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
@@ -39258,10 +39408,10 @@
       <c r="F10" s="19"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
         <v>38</v>
       </c>
@@ -39272,7 +39422,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
@@ -39281,25 +39431,25 @@
       <c r="F13" s="18"/>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="18"/>
       <c r="D14" s="20"/>
       <c r="F14" s="18"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="18"/>
       <c r="D15" s="20"/>
       <c r="F15" s="18"/>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="18"/>
       <c r="D16" s="20"/>
       <c r="F16" s="18"/>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="18"/>
       <c r="D17" s="20"/>
       <c r="F17" s="18"/>
@@ -39335,18 +39485,18 @@
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
@@ -39366,19 +39516,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
@@ -39394,38 +39544,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="3" width="4.1328125" customWidth="1"/>
-    <col min="13" max="13" width="16.73046875" customWidth="1"/>
-    <col min="14" max="14" width="21.265625" customWidth="1"/>
-    <col min="15" max="15" width="33.86328125" customWidth="1"/>
-    <col min="16" max="16" width="48.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.28515625" customWidth="1"/>
+    <col min="15" max="15" width="33.85546875" customWidth="1"/>
+    <col min="16" max="16" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M5" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M6" s="11"/>
       <c r="N6" s="11" t="s">
         <v>52</v>
@@ -39437,7 +39587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
@@ -39452,7 +39602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N8" t="s">
         <v>59</v>
       </c>
@@ -39460,12 +39610,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M11" s="13" t="s">
         <v>62</v>
       </c>
@@ -39479,7 +39629,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N12" s="17" t="s">
         <v>69</v>
       </c>
@@ -39490,7 +39640,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M14" s="13" t="s">
         <v>55</v>
       </c>
@@ -39504,7 +39654,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="O15" s="16" t="s">
         <v>105</v>
       </c>
@@ -39512,7 +39662,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
       <c r="M17" s="13" t="s">
         <v>65</v>
       </c>
@@ -39526,7 +39676,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
       <c r="M19" s="13" t="s">
         <v>56</v>
@@ -39541,7 +39691,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="N20" t="s">
         <v>67</v>
       </c>
@@ -39552,12 +39702,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="N21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="N22" t="s">
         <v>69</v>
       </c>
@@ -39580,24 +39730,24 @@
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="Q2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:21" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:21" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -39605,13 +39755,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="Q4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>20</v>
       </c>
@@ -39619,7 +39769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>21</v>
       </c>
@@ -39627,7 +39777,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>22</v>
       </c>
@@ -39635,7 +39785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>26</v>
       </c>
@@ -39643,7 +39793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="R10" t="s">
         <v>28</v>
       </c>
@@ -39651,67 +39801,67 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="51" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="55" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="56" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P56" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="57" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="58" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="61" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="63" spans="15:16" x14ac:dyDescent="0.25">
       <c r="O63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="15:16" x14ac:dyDescent="0.45">
+    <row r="64" spans="15:16" x14ac:dyDescent="0.25">
       <c r="P64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.45">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P65" t="s">
         <v>50</v>
       </c>
@@ -39731,79 +39881,79 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.73046875" style="1"/>
-    <col min="4" max="4" width="32.3984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.73046875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.73046875" style="1"/>
-    <col min="8" max="8" width="43.86328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.73046875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.73046875" style="1" customWidth="1"/>
-    <col min="11" max="16" width="10.73046875" style="1"/>
-    <col min="17" max="19" width="5.86328125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.59765625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.59765625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.86328125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.265625" style="1" customWidth="1"/>
-    <col min="24" max="26" width="10.73046875" style="1"/>
-    <col min="27" max="27" width="13.59765625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="10.73046875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="32.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="1"/>
+    <col min="8" max="8" width="43.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16" width="10.7109375" style="1"/>
+    <col min="17" max="19" width="5.85546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="1" customWidth="1"/>
+    <col min="24" max="26" width="10.7109375" style="1"/>
+    <col min="27" max="27" width="13.5703125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.7109375" style="1"/>
     <col min="29" max="29" width="12" style="1" customWidth="1"/>
-    <col min="30" max="37" width="10.73046875" style="1"/>
+    <col min="30" max="37" width="10.7109375" style="1"/>
     <col min="38" max="38" width="16" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="10.73046875" style="1"/>
+    <col min="39" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:33" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.65">
+    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AG7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
       <c r="AG12" s="1" t="s">
         <v>14</v>
       </c>
@@ -39823,156 +39973,156 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
     </row>
-    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="14:15" x14ac:dyDescent="0.25">
       <c r="N38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="14:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="14:15" x14ac:dyDescent="0.25">
       <c r="O42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="T85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U86" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U87" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U88" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="U89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G175" t="s">
         <v>4</v>
       </c>
@@ -39992,18 +40142,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.265625" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Regel für SQL Agent Benutzer ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05587397-1CA5-46E4-A8D5-EF8A1B095C46}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A645D3F9-F50F-42A7-AC47-6DEAEE26B892}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,8 +677,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -14231,15 +14231,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14254,8 +14254,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3810000" y="6410325"/>
-          <a:ext cx="1857375" cy="638175"/>
+          <a:off x="4057650" y="6515100"/>
+          <a:ext cx="1971675" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14337,8 +14337,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -14353,8 +14353,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3781424" y="5553075"/>
-          <a:ext cx="4695825" cy="762000"/>
+          <a:off x="4038599" y="5305425"/>
+          <a:ext cx="5038725" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14437,6 +14437,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="de-DE" sz="800" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>User des SQL Agent (Domäne\Server$) in DataFactory als User berechtigen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="de-DE" sz="800">
             <a:solidFill>
               <a:srgbClr val="203864"/>
@@ -14881,16 +14898,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>771526</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>459457</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>297532</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14919,8 +14936,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2828926" y="6391275"/>
-          <a:ext cx="345156" cy="323850"/>
+          <a:off x="2867026" y="2762250"/>
+          <a:ext cx="345156" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -38982,273 +38999,273 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C6" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D7" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D9" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D10" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C12" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D13" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D14" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D15" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D16" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D17" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D18" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C20" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D21" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="10"/>
       <c r="D25" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="10"/>
       <c r="D26" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" s="10"/>
       <c r="D27" s="14"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C28" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D29" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D35" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C37" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D38" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C40" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D41" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D42" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D43" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D44" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.45">
       <c r="C46" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D47" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.45">
       <c r="D48" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D49" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D50" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D51" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D52" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C54" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D55" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D56" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D57" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B60" s="10" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
       <c r="C61" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D62" s="1" t="s">
         <v>94</v>
       </c>
@@ -39268,18 +39285,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
@@ -39298,18 +39315,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7"/>
     </row>
   </sheetData>
@@ -39326,18 +39343,18 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>30</v>
       </c>
@@ -39356,62 +39373,62 @@
       <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B9" s="8"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C12" s="8" t="s">
         <v>38</v>
       </c>
@@ -39422,41 +39439,46 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="19"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="19"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="19"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C15" s="18"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="19"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
       <c r="C16" s="18"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="19"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C17" s="18"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="19"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C13:D13"/>
@@ -39465,11 +39487,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39485,18 +39502,18 @@
       <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>32</v>
       </c>
@@ -39516,19 +39533,19 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>75</v>
       </c>
@@ -39545,37 +39562,37 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="4.140625" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1"/>
-    <col min="15" max="15" width="33.85546875" customWidth="1"/>
-    <col min="16" max="16" width="48.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="3" width="4.1328125" customWidth="1"/>
+    <col min="13" max="13" width="16.73046875" customWidth="1"/>
+    <col min="14" max="14" width="21.265625" customWidth="1"/>
+    <col min="15" max="15" width="33.86328125" customWidth="1"/>
+    <col min="16" max="16" width="48.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.45">
       <c r="M5" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
       <c r="M6" s="11"/>
       <c r="N6" s="11" t="s">
         <v>52</v>
@@ -39587,7 +39604,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.45">
       <c r="E7" s="3"/>
       <c r="M7" s="13" t="s">
         <v>57</v>
@@ -39602,7 +39619,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
       <c r="N8" t="s">
         <v>59</v>
       </c>
@@ -39610,12 +39627,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
       <c r="N9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
       <c r="M11" s="13" t="s">
         <v>62</v>
       </c>
@@ -39629,7 +39646,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.45">
       <c r="N12" s="17" t="s">
         <v>69</v>
       </c>
@@ -39640,7 +39657,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
       <c r="M14" s="13" t="s">
         <v>55</v>
       </c>
@@ -39654,7 +39671,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
       <c r="O15" s="16" t="s">
         <v>105</v>
       </c>
@@ -39662,7 +39679,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:16" x14ac:dyDescent="0.45">
       <c r="M17" s="13" t="s">
         <v>65</v>
       </c>
@@ -39676,7 +39693,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:16" x14ac:dyDescent="0.45">
       <c r="D19" s="4"/>
       <c r="M19" s="13" t="s">
         <v>56</v>
@@ -39691,7 +39708,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.45">
       <c r="N20" t="s">
         <v>67</v>
       </c>
@@ -39702,12 +39719,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:16" x14ac:dyDescent="0.45">
       <c r="N21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.45">
       <c r="N22" t="s">
         <v>69</v>
       </c>
@@ -39730,24 +39747,24 @@
       <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7"/>
       <c r="Q2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:21" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:21" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -39755,13 +39772,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
       <c r="B4" s="2"/>
       <c r="Q4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.45">
       <c r="R6" t="s">
         <v>20</v>
       </c>
@@ -39769,7 +39786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.45">
       <c r="R7" t="s">
         <v>21</v>
       </c>
@@ -39777,7 +39794,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.45">
       <c r="R8" t="s">
         <v>22</v>
       </c>
@@ -39785,7 +39802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.45">
       <c r="R9" t="s">
         <v>26</v>
       </c>
@@ -39793,7 +39810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.45">
       <c r="R10" t="s">
         <v>28</v>
       </c>
@@ -39801,67 +39818,67 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="15:15" x14ac:dyDescent="0.45">
       <c r="O48" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="15:16" x14ac:dyDescent="0.45">
       <c r="O54" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P56" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="15:16" x14ac:dyDescent="0.45">
       <c r="O61" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="15:16" x14ac:dyDescent="0.45">
       <c r="O63" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="15:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="15:16" x14ac:dyDescent="0.45">
       <c r="P64" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.45">
       <c r="P65" t="s">
         <v>50</v>
       </c>
@@ -39881,79 +39898,79 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" style="1"/>
-    <col min="4" max="4" width="32.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="1"/>
-    <col min="8" max="8" width="43.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="1" customWidth="1"/>
-    <col min="11" max="16" width="10.7109375" style="1"/>
-    <col min="17" max="19" width="5.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" style="1" customWidth="1"/>
-    <col min="24" max="26" width="10.7109375" style="1"/>
-    <col min="27" max="27" width="13.5703125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="2.265625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.73046875" style="1"/>
+    <col min="4" max="4" width="32.3984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.73046875" style="1"/>
+    <col min="8" max="8" width="43.86328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" style="1" customWidth="1"/>
+    <col min="11" max="16" width="10.73046875" style="1"/>
+    <col min="17" max="19" width="5.86328125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.59765625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.59765625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.86328125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="15.265625" style="1" customWidth="1"/>
+    <col min="24" max="26" width="10.73046875" style="1"/>
+    <col min="27" max="27" width="13.59765625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.73046875" style="1"/>
     <col min="29" max="29" width="12" style="1" customWidth="1"/>
-    <col min="30" max="37" width="10.7109375" style="1"/>
+    <col min="30" max="37" width="10.73046875" style="1"/>
     <col min="38" max="38" width="16" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="10.7109375" style="1"/>
+    <col min="39" max="16384" width="10.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:33" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:33" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:33" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:33" ht="21" x14ac:dyDescent="0.65">
       <c r="B4" s="2"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" ht="81.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="AG7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
       <c r="AG12" s="1" t="s">
         <v>14</v>
       </c>
@@ -39973,156 +39990,156 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.65">
       <c r="B3" s="2"/>
     </row>
-    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="11" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="14" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="14:14" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="31" spans="14:14" x14ac:dyDescent="0.45">
       <c r="N31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="14:15" x14ac:dyDescent="0.45">
       <c r="N38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:15" x14ac:dyDescent="0.45">
       <c r="O39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="14:15" x14ac:dyDescent="0.45">
       <c r="O40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:15" x14ac:dyDescent="0.45">
       <c r="O41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:15" x14ac:dyDescent="0.45">
       <c r="O42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="82" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="84" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="T85" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="U86" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="U87" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="U88" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="U89" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="91" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="92" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="93" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="94" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="95" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="96" spans="20:21" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="175" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G175" t="s">
         <v>4</v>
       </c>
@@ -40142,18 +40159,18 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B1" s="9" t="str">
         <f>lblAuftraggeber</f>
         <v>Musterfirma</v>
       </c>
     </row>
-    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:2" s="6" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Regel für Deployment XLS Client
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
+++ b/8. Harmonising standards/Create a project/Vorlage Betriebsdokumentation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A67678-7E00-419B-9BA4-FFCFB4B0E728}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6DE5E3-E6D8-4B79-9172-0F566A52DE70}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -677,8 +677,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -15268,6 +15268,208 @@
               </a:solidFill>
             </a:rPr>
             <a:t>Schreibrechte für Domäne\saxess</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:srgbClr val="203864"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>770407</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>153106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Grafik 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD56234-9D53-4AB2-B19C-6CAF88257A91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8963025" y="6896100"/>
+          <a:ext cx="2389657" cy="1839031"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>892950</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>334709</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>83562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Grafik 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5D414B-C805-43AF-AA26-8EB77F48BC5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8941575" y="6086475"/>
+          <a:ext cx="4232834" cy="864612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Textfeld 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69431634-B792-4356-A9F1-46F8AC1FC3AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9029700" y="5476875"/>
+          <a:ext cx="2771776" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Excel Client generisch benannt auf Netzlaufwerk</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> ablegen.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="0" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="203864"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Ordner und Daten umbenennen um diese Namen bei Updates konstant zu halten.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -39739,20 +39941,20 @@
       <c r="C4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -39762,10 +39964,10 @@
         <v>36</v>
       </c>
       <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
@@ -39786,36 +39988,41 @@
         <v>37</v>
       </c>
       <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
+      <c r="D13" s="19"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C14" s="18"/>
-      <c r="D14" s="20"/>
+      <c r="D14" s="19"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="20"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C15" s="18"/>
-      <c r="D15" s="20"/>
+      <c r="D15" s="19"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="20"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="18"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="19"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="20"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="18"/>
-      <c r="D17" s="20"/>
+      <c r="D17" s="19"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="20"/>
+      <c r="G17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="C13:D13"/>
@@ -39824,11 +40031,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39903,8 +40105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>